<commit_message>
commit for scan 22/7/2024
</commit_message>
<xml_diff>
--- a/digiverifier_backened/src/main/resources/conventional_candidate.xlsx
+++ b/digiverifier_backened/src/main/resources/conventional_candidate.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nambi\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nambi\git\Digiverifier-New\Digiverifier-New_Hybrid\project\digiverifier_backend\digiverifier\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD7A3575-6CD4-4FBA-9CC8-4837CA72EB60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F7DFAE1-7D46-446C-8E2F-70111C5170D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -567,12 +567,15 @@
       <c r="B9" s="2"/>
     </row>
   </sheetData>
-  <dataValidations count="2">
+  <dataValidations count="3">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2" xr:uid="{4CAFC8F9-FE83-4AA4-8D20-CCC2580C3168}">
       <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F181" xr:uid="{1E6DF708-0446-458F-AD0D-F4E644E28F14}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3:F181" xr:uid="{1E6DF708-0446-458F-AD0D-F4E644E28F14}">
       <formula1>"BT,CTL,Verizon,Standard 1 with Criminal"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2" xr:uid="{205CFA49-D706-4CAD-B14A-B29C05CB653C}">
+      <formula1>"BT,CTL,Verizon,Standard 1 with Criminal,Verizon (Existing-Employee)"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>

</xml_diff>